<commit_message>
C# Final Project Draft
</commit_message>
<xml_diff>
--- a/CSharpFinalAssignment/ExcelReference.xlsx
+++ b/CSharpFinalAssignment/ExcelReference.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharath\Documents\GitHub\TechAcademy-CSharp-Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharath\Documents\GitHub\TechAcademy-CSharp-Final\CSharpFinalAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ADE632-35FC-4E65-B65C-F294B9602DED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CCBF33-49B7-4D97-AA0E-868BDD330066}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4763EE0-EBFA-40EE-9489-66A3FFFA0F9D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Barack</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>William (Bill)</t>
+  </si>
+  <si>
+    <t>Calvin</t>
+  </si>
+  <si>
+    <t>Coolidge</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -463,21 +475,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0522FED4-A3DF-41E1-81B1-069B628FFB7F}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="2" max="3" width="11.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,22 +497,25 @@
         <v>1</v>
       </c>
       <c r="C1">
+        <v>44</v>
+      </c>
+      <c r="D1">
         <v>1961</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2009</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2017</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -508,22 +523,25 @@
         <v>11</v>
       </c>
       <c r="C2">
+        <v>43</v>
+      </c>
+      <c r="D2">
         <v>1946</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2001</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2009</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -531,22 +549,25 @@
         <v>12</v>
       </c>
       <c r="C3">
+        <v>42</v>
+      </c>
+      <c r="D3">
         <v>1946</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1993</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2001</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -554,22 +575,25 @@
         <v>13</v>
       </c>
       <c r="C4">
+        <v>41</v>
+      </c>
+      <c r="D4">
         <v>1924</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1989</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1993</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -577,22 +601,25 @@
         <v>14</v>
       </c>
       <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
         <v>1911</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1981</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1989</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -600,22 +627,25 @@
         <v>15</v>
       </c>
       <c r="C6">
+        <v>39</v>
+      </c>
+      <c r="D6">
         <v>1924</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1977</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1981</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -623,22 +653,25 @@
         <v>16</v>
       </c>
       <c r="C7">
+        <v>38</v>
+      </c>
+      <c r="D7">
         <v>1813</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1974</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1977</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -646,22 +679,25 @@
         <v>17</v>
       </c>
       <c r="C8">
+        <v>37</v>
+      </c>
+      <c r="D8">
         <v>1913</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1969</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1974</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -669,22 +705,25 @@
         <v>18</v>
       </c>
       <c r="C9">
+        <v>36</v>
+      </c>
+      <c r="D9">
         <v>1908</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1963</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>1969</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -692,22 +731,25 @@
         <v>19</v>
       </c>
       <c r="C10">
+        <v>35</v>
+      </c>
+      <c r="D10">
         <v>1917</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1961</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>1963</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -715,22 +757,25 @@
         <v>20</v>
       </c>
       <c r="C11">
+        <v>34</v>
+      </c>
+      <c r="D11">
         <v>1890</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1953</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>1961</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>25</v>
       </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -738,22 +783,25 @@
         <v>23</v>
       </c>
       <c r="C12">
+        <v>33</v>
+      </c>
+      <c r="D12">
         <v>1884</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1945</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>1953</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -761,22 +809,25 @@
         <v>22</v>
       </c>
       <c r="C13">
+        <v>32</v>
+      </c>
+      <c r="D13">
         <v>1882</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>1933</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>1945</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>24</v>
       </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -784,19 +835,48 @@
         <v>21</v>
       </c>
       <c r="C14">
+        <v>31</v>
+      </c>
+      <c r="D14">
         <v>1874</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>1929</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>1933</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="b">
-        <v>0</v>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>1872</v>
+      </c>
+      <c r="E15">
+        <v>1923</v>
+      </c>
+      <c r="F15">
+        <v>1929</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>